<commit_message>
Sprint 3 US04 & US34
US04 & US34  done by lingwen kong
</commit_message>
<xml_diff>
--- a/Report backlog_and_teamsheet.xlsx
+++ b/Report backlog_and_teamsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubrey/PycharmProjects/SSW-555-A-Project-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasir\Desktop\september\python-assignment\github\Project3\SSW-555-A-Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED6CDF7-25D3-3F41-B774-D0DDB4821A16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7048B5C0-EF60-4AEA-875C-EC070867524F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="201">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -535,7 +526,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -735,20 +726,53 @@
     <t xml:space="preserve"> List all people in a GEDCOM file who were born in the last 30 days</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>US34</t>
+  </si>
+  <si>
+    <t>List large age difference</t>
+  </si>
+  <si>
+    <t>US04</t>
+  </si>
+  <si>
+    <t>Marriage before divorce</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> List all people in a GEDCOM file who are spouses with large age difference</t>
+  </si>
+  <si>
+    <t>T34.01</t>
+  </si>
+  <si>
+    <t>T34.02</t>
+  </si>
+  <si>
+    <t>marriage before divorce</t>
+  </si>
+  <si>
+    <t>T04.01</t>
+  </si>
+  <si>
+    <t>T04.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> List all people in a GEDCOM file with marriage before divorce</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -760,7 +784,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -774,14 +798,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -789,14 +813,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0066CC"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -810,7 +834,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -830,7 +854,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -839,7 +863,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -847,7 +871,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -875,7 +899,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -891,23 +915,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -934,9 +959,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{0806C502-5B25-4AE5-A7E3-7A9818F2DFE2}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -954,7 +979,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1394,10 +1419,10 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1507,17 +1532,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C06F4B-E189-4612-9398-61FC56C851BF}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1944,6 +1969,40 @@
       </c>
       <c r="E27" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="22">
+        <v>3</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1961,16 +2020,16 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="8"/>
-    <col min="2" max="2" width="20.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="8"/>
+    <col min="2" max="2" width="20.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="12.5" style="8"/>
+    <col min="4" max="4" width="14.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="12.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2104,24 +2163,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7423B761-4644-4B14-9E93-F056AD5F843E}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.83203125" customWidth="1"/>
+    <col min="13" max="13" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.5" customHeight="1">
+    <row r="1" spans="1:13" ht="18.600000000000001" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2178,18 +2237,18 @@
       <c r="I2" s="15">
         <v>44272</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" t="s">
@@ -2201,11 +2260,11 @@
       <c r="C4" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" t="s">
@@ -2217,13 +2276,13 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-    </row>
-    <row r="6" spans="1:13" ht="16">
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2233,14 +2292,14 @@
       <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -2267,20 +2326,20 @@
       <c r="I8" s="15">
         <v>44272</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-    </row>
-    <row r="10" spans="1:13" ht="16">
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2293,13 +2352,13 @@
       <c r="D10" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="1:13" ht="16">
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2310,7 +2369,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2322,13 +2381,13 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-    </row>
-    <row r="14" spans="1:13" ht="16">
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2356,14 +2415,14 @@
       <c r="I14" s="15">
         <v>44258</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="25">
         <f>SUM(H:H)</f>
         <v>230</v>
       </c>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-    </row>
-    <row r="16" spans="1:13" ht="16">
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2684,15 +2743,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7481DEDB-4C58-7441-A282-5807B9B53AF9}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="57.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="16" max="16" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -2752,21 +2811,21 @@
       <c r="I2" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
@@ -2778,14 +2837,14 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
@@ -2797,14 +2856,14 @@
       <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
@@ -2829,14 +2888,14 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
@@ -2866,24 +2925,24 @@
       <c r="I9" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
@@ -2917,22 +2976,22 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="6" t="s">
@@ -2945,7 +3004,7 @@
         <v>67</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E15" s="16">
         <v>30</v>
@@ -3022,7 +3081,7 @@
         <v>67</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E20" s="16">
         <v>25</v>
@@ -3146,16 +3205,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEB31C5-8FAF-D54E-8C1E-527269570479}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="53.5" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3300,6 +3359,154 @@
         <v>44</v>
       </c>
     </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="22">
+        <v>100</v>
+      </c>
+      <c r="F14" s="22">
+        <v>120</v>
+      </c>
+      <c r="G14" s="22">
+        <v>20</v>
+      </c>
+      <c r="H14" s="22">
+        <v>100</v>
+      </c>
+      <c r="I14" s="21">
+        <v>44299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="22">
+        <v>100</v>
+      </c>
+      <c r="F19" s="22">
+        <v>120</v>
+      </c>
+      <c r="G19" s="22">
+        <v>40</v>
+      </c>
+      <c r="H19" s="22">
+        <v>90</v>
+      </c>
+      <c r="I19" s="21">
+        <v>44299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>